<commit_message>
rename the template file modify sheetname for coverage group
</commit_message>
<xml_diff>
--- a/AHB_M_COV.xlsx
+++ b/AHB_M_COV.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="cg_AAA" sheetId="1" r:id="rId1"/>
+    <sheet name="cg_ahb_master" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
@@ -837,8 +837,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D57" sqref="D57"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="G59" sqref="G59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.4"/>

</xml_diff>